<commit_message>
mini v2 and added parameterization of v2
</commit_message>
<xml_diff>
--- a/parameter_files/v2/sigmas.xlsx
+++ b/parameter_files/v2/sigmas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4efc3e9dc81381f4/Documents/SJV-gen-modeling/parameter_files/v2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{4086C040-E826-4301-AC05-6166F276BF61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9C73BE6-43EA-41C5-8859-C548E6490AE1}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{4086C040-E826-4301-AC05-6166F276BF61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC45B886-5013-4477-A21B-1F6245872331}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1219,10 +1219,10 @@
   <dimension ref="A1:AJ36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="V14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="Q11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W40" sqref="W40"/>
+      <selection pane="bottomRight" activeCell="W24" sqref="W24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1771,6 +1771,9 @@
       <c r="T22">
         <v>1</v>
       </c>
+      <c r="W22">
+        <v>0.5</v>
+      </c>
       <c r="AI22" s="5">
         <v>2</v>
       </c>
@@ -1785,6 +1788,9 @@
       <c r="B23" s="4"/>
       <c r="H23" s="5"/>
       <c r="R23" s="4"/>
+      <c r="V23">
+        <v>0.5</v>
+      </c>
       <c r="AI23" s="5"/>
     </row>
     <row r="24" spans="1:36" x14ac:dyDescent="0.35">

</xml_diff>